<commit_message>
added table on paper 3
</commit_message>
<xml_diff>
--- a/Lab_1/Tables.xlsx
+++ b/Lab_1/Tables.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucadipietro/Desktop/UNI/Erasmus/EHC/EHCLab/Lab_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E42C1F69-3259-034F-A1A5-F1471C53DD5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74023E8C-1CB9-0B44-AD27-456C4DC482FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16020" xr2:uid="{7C8710E0-D4D5-E54E-A4BB-E37F4F498C84}"/>
+    <workbookView xWindow="10600" yWindow="1720" windowWidth="20960" windowHeight="14240" activeTab="2" xr2:uid="{7C8710E0-D4D5-E54E-A4BB-E37F4F498C84}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
     <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
+    <sheet name="Foglio3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Colonna1</t>
   </si>
@@ -112,19 +113,123 @@
   </si>
   <si>
     <t>Colonna9</t>
+  </si>
+  <si>
+    <t>Option</t>
+  </si>
+  <si>
+    <t>EDP (ExD)</t>
+  </si>
+  <si>
+    <r>
+      <t>ED</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>P (ExDxD)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ED</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Corpo)"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>P (ExDxDxD)</t>
+    </r>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>I</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow (Corpo)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -156,7 +261,10 @@
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -195,15 +303,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9D23C27B-6488-FB4D-9FC9-48B3A95E9DE5}" name="Table_1" displayName="Table_1" ref="B3:G4" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9D23C27B-6488-FB4D-9FC9-48B3A95E9DE5}" name="Table_1" displayName="Table_1" ref="B3:G4" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="B3:G4" xr:uid="{9D23C27B-6488-FB4D-9FC9-48B3A95E9DE5}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{6A4FAB3C-B8F8-3A49-BF6F-79D6A8168240}" name="CPU used" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{9C20290B-E119-9C40-8E13-B2C69BE20D57}" name="#Phisical cores" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{2A7CB0DE-FA62-6A44-9E86-28BCD48D6251}" name="#Logical  cores" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{37845CFA-E711-524E-93B3-F29EBE6D3BCD}" name="Max Clock Frequency" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{7563A5EC-8567-2F45-93B0-BCC0B6C90343}" name="Size of caches" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{BBDE40D3-39DD-1E44-BAE7-C48520481250}" name="Size of physical memory" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{6A4FAB3C-B8F8-3A49-BF6F-79D6A8168240}" name="CPU used" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{9C20290B-E119-9C40-8E13-B2C69BE20D57}" name="#Phisical cores" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{2A7CB0DE-FA62-6A44-9E86-28BCD48D6251}" name="#Logical  cores" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{37845CFA-E711-524E-93B3-F29EBE6D3BCD}" name="Max Clock Frequency" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{7563A5EC-8567-2F45-93B0-BCC0B6C90343}" name="Size of caches" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{BBDE40D3-39DD-1E44-BAE7-C48520481250}" name="Size of physical memory" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -234,6 +342,19 @@
     <tableColumn id="7" xr3:uid="{47804360-C00C-EB41-ACB4-9D3382A8DBFE}" name="Colonna7"/>
     <tableColumn id="8" xr3:uid="{F7F48973-483E-0B4F-A0DF-BADCAA1EC4E8}" name="Colonna8"/>
     <tableColumn id="9" xr3:uid="{0FCA2E73-808A-4541-B23C-83EA6C7664D3}" name="Colonna9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3C85B5C2-E3B6-0148-80A3-752F04DCCA0D}" name="Tabella3" displayName="Tabella3" ref="A1:D13" totalsRowShown="0">
+  <autoFilter ref="A1:D13" xr:uid="{3C85B5C2-E3B6-0148-80A3-752F04DCCA0D}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{7198354A-E1DF-6140-829E-102C9FAC6201}" name="Option" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{2D52263B-C1F5-6C46-8746-E9EFF5373C9C}" name="EDP (ExD)"/>
+    <tableColumn id="3" xr3:uid="{7BBF4155-5EE9-AF48-9B67-65DA0C896F31}" name="ED2P (ExDxD)"/>
+    <tableColumn id="4" xr3:uid="{6A00F963-8B4E-294B-9352-D7492B804A89}" name="ED3P (ExDxDxD)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -558,7 +679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE2BB4C-8B45-E14E-BB9C-83126F32B72A}">
   <dimension ref="B3:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -693,4 +814,102 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59113A16-097B-FF47-B268-BA291D7DA61F}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>